<commit_message>
Modificado numero de Vela Duarte Argerich
</commit_message>
<xml_diff>
--- a/ILCA RADIAL.xlsx
+++ b/ILCA RADIAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Desktop\SIY ILCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9002897-310C-4121-B017-797E7C1AA59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E30CD4D-03BC-4EA8-BC34-3D61FCF59FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="194">
   <si>
     <t>Club</t>
   </si>
@@ -986,6 +986,9 @@
   </si>
   <si>
     <t>CHI</t>
+  </si>
+  <si>
+    <t>111</t>
   </si>
 </sst>
 </file>
@@ -1384,8 +1387,8 @@
   <dimension ref="A1:O81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2268,7 +2271,7 @@
         <v>8</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>110</v>
+        <v>193</v>
       </c>
       <c r="D40" s="7">
         <v>35446</v>

</xml_diff>